<commit_message>
Tweaked on the excel sheet a bit because something was wrong
</commit_message>
<xml_diff>
--- a/Oracle/Assignment 4/IS-309 A4 Excel.xlsx
+++ b/Oracle/Assignment 4/IS-309 A4 Excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CCE22-86A5-6C44-AA1E-892642AD685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A231FA82-95B2-4DE6-BFA7-FE9365B6E446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="450" windowWidth="30150" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Uprise Art" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Table</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>NEXT extent size (MB)</t>
+  </si>
+  <si>
+    <t>Size for one year</t>
+  </si>
+  <si>
+    <t>Tablespace</t>
+  </si>
+  <si>
+    <t>BCYCLE64K</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -202,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -240,6 +252,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -247,7 +270,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -288,6 +311,9 @@
     <xf numFmtId="3" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -318,94 +344,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1704975</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>208895</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>28088</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Bilde 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D6B1E8B-7980-4F83-902A-DF79AAA6C499}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="24374475" y="4895850"/>
-          <a:ext cx="5238095" cy="3895238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>1580494</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>37606</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Bilde 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3217848C-9642-4D90-97E3-F96FBAA6654C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19011900" y="4848225"/>
-          <a:ext cx="5238095" cy="3952381"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>20</xdr:row>
@@ -431,7 +369,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -440,6 +378,50 @@
         <a:xfrm>
           <a:off x="8134350" y="4305300"/>
           <a:ext cx="10676190" cy="6114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>940002</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>46548</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>387789</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>170119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Bilde 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43FFE3A9-7CF0-40A0-8CE2-36BA263F335C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19088790" y="4428048"/>
+          <a:ext cx="9500326" cy="2028571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -772,38 +754,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.83203125" customWidth="1"/>
-    <col min="8" max="8" width="19.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="14.83203125" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.83203125" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -852,8 +835,14 @@
       <c r="P1" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>19</v>
       </c>
@@ -911,8 +900,15 @@
         <f>O2/1024</f>
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <f>O2+(2*P2)</f>
+        <v>65664</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>20</v>
       </c>
@@ -972,8 +968,12 @@
         <f t="shared" ref="P3:P11" si="5">O3/1024</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <f>O3+(2*P3)</f>
+        <v>128.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
@@ -1033,8 +1033,12 @@
         <f t="shared" si="5"/>
         <v>16384</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <f>O4+(2*P4)</f>
+        <v>16809984</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>22</v>
       </c>
@@ -1088,8 +1092,12 @@
         <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" t="e">
+        <f>O5+(2*P5)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
@@ -1149,8 +1157,12 @@
         <f t="shared" si="5"/>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <f>O6+(2*P6)</f>
+        <v>128.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
@@ -1210,8 +1222,12 @@
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <f>O7+(2*P7)</f>
+        <v>32832</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
@@ -1229,8 +1245,8 @@
         <v>0</v>
       </c>
       <c r="F8" s="16">
-        <f>F10*3</f>
-        <v>97200</v>
+        <f>F9*3</f>
+        <v>1944</v>
       </c>
       <c r="G8" s="16">
         <f>G9*3</f>
@@ -1245,11 +1261,11 @@
       </c>
       <c r="J8" s="18">
         <f t="shared" si="1"/>
-        <v>19245600</v>
+        <v>384912.00000000006</v>
       </c>
       <c r="K8" s="20">
         <f t="shared" si="2"/>
-        <v>18794.53125</v>
+        <v>375.89062500000006</v>
       </c>
       <c r="L8" s="21">
         <f t="shared" si="7"/>
@@ -1261,7 +1277,7 @@
       </c>
       <c r="N8" s="22">
         <f t="shared" si="4"/>
-        <v>18816</v>
+        <v>384</v>
       </c>
       <c r="O8" s="24" t="str">
         <f t="shared" si="8"/>
@@ -1271,8 +1287,12 @@
         <f t="shared" si="5"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <f>O8+(2*P8)</f>
+        <v>64.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>26</v>
       </c>
@@ -1330,8 +1350,12 @@
         <f t="shared" si="5"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <f>O9+(2*P9)</f>
+        <v>64.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>27</v>
       </c>
@@ -1391,8 +1415,12 @@
         <f t="shared" si="5"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <f>O10+(2*P10)</f>
+        <v>64.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>28</v>
       </c>
@@ -1452,8 +1480,12 @@
         <f t="shared" si="5"/>
         <v>8192</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q11">
+        <f>O11+(2*P11)</f>
+        <v>8404992</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="5"/>
@@ -1463,7 +1495,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="K13" s="2"/>
@@ -1471,13 +1503,13 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K14" s="2"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>3</v>
       </c>
@@ -1494,7 +1526,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="K16" s="2"/>
@@ -1502,7 +1534,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="K17" s="2"/>
@@ -1510,7 +1542,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="K18" s="2"/>
@@ -1518,84 +1550,89 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="M19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
+    </row>
+    <row r="42" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>